<commit_message>
add load_xlsx get correlation data
</commit_message>
<xml_diff>
--- a/loader/test/building.xlsx
+++ b/loader/test/building.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>建筑标识</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>嗯嗯嗯嗯呃呃123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userlevel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关联userlevel表主键</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -109,15 +121,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,13 +143,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -414,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -425,193 +464,224 @@
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="10.75" customWidth="1"/>
+    <col min="6" max="6" width="18.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>1000</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>100</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>-200</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>1001</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>100</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>-200</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="F5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>1002</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>100</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>-200</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>1003</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>1001</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>-2002</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="F7" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>1004</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>100</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>-200</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>1005</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>100</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
         <v>-200</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="F9" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>1006</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>100</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
         <v>-200</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>

</xml_diff>